<commit_message>
Remoção dos scripts .py
</commit_message>
<xml_diff>
--- a/scripts/Modelo_2sections.xlsx
+++ b/scripts/Modelo_2sections.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="EstaPasta_de_trabalho" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hr7o\Documents\Portable Git\ccp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hr7o\Documents\Portable Git\ccp\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -4693,6 +4693,66 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="14" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="15" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="15" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="15" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="16" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="3" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="3" borderId="15" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="3" borderId="16" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="22" fillId="5" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="22" fillId="5" borderId="15" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="22" fillId="5" borderId="16" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="22" fillId="0" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="22" fillId="0" borderId="15" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="22" fillId="0" borderId="16" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="3" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4704,66 +4764,6 @@
     </xf>
     <xf numFmtId="164" fontId="11" fillId="3" borderId="15" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="3" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="3" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="3" borderId="14" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="3" borderId="15" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="3" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="15" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="15" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="16" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="15" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="16" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="22" fillId="5" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="22" fillId="5" borderId="15" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="22" fillId="5" borderId="16" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="22" fillId="0" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="22" fillId="0" borderId="15" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="22" fillId="0" borderId="16" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="3" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -6044,7 +6044,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6993,7 +6992,6 @@
         <c:idx val="1"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7105,7 +7103,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7741,7 +7738,6 @@
         <c:idx val="1"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -17807,7 +17803,7 @@
   <dimension ref="A1:AX175"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="T24" sqref="T24:V24"/>
+      <selection activeCell="T36" sqref="T36:V36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19040,11 +19036,11 @@
       </c>
       <c r="X21" s="476"/>
       <c r="Y21" s="477"/>
-      <c r="Z21" s="447">
+      <c r="Z21" s="443">
         <v>282554</v>
       </c>
-      <c r="AA21" s="448"/>
-      <c r="AB21" s="449"/>
+      <c r="AA21" s="444"/>
+      <c r="AB21" s="445"/>
       <c r="AC21" s="478"/>
       <c r="AD21" s="479"/>
       <c r="AE21" s="480"/>
@@ -19150,22 +19146,22 @@
       <c r="Q23" s="13"/>
       <c r="R23" s="13"/>
       <c r="S23" s="13"/>
-      <c r="T23" s="447">
+      <c r="T23" s="443">
         <v>1.6995</v>
       </c>
-      <c r="U23" s="448"/>
-      <c r="V23" s="449"/>
+      <c r="U23" s="444"/>
+      <c r="V23" s="445"/>
       <c r="W23" s="388"/>
       <c r="X23" s="389"/>
       <c r="Y23" s="390"/>
-      <c r="Z23" s="447">
+      <c r="Z23" s="443">
         <v>3.4830000000000001</v>
       </c>
-      <c r="AA23" s="448"/>
-      <c r="AB23" s="449"/>
-      <c r="AC23" s="450"/>
-      <c r="AD23" s="451"/>
-      <c r="AE23" s="452"/>
+      <c r="AA23" s="444"/>
+      <c r="AB23" s="445"/>
+      <c r="AC23" s="446"/>
+      <c r="AD23" s="447"/>
+      <c r="AE23" s="448"/>
       <c r="AF23" s="44"/>
       <c r="AG23" s="44"/>
       <c r="AH23" s="44"/>
@@ -19213,24 +19209,24 @@
       <c r="Q24" s="13"/>
       <c r="R24" s="13"/>
       <c r="S24" s="13"/>
-      <c r="T24" s="447">
+      <c r="T24" s="443">
         <v>-23.914999999999999</v>
       </c>
-      <c r="U24" s="448"/>
-      <c r="V24" s="449"/>
-      <c r="W24" s="447">
+      <c r="U24" s="444"/>
+      <c r="V24" s="445"/>
+      <c r="W24" s="443">
         <v>-1.1499999999999999</v>
       </c>
-      <c r="X24" s="448"/>
-      <c r="Y24" s="449"/>
-      <c r="Z24" s="447">
+      <c r="X24" s="444"/>
+      <c r="Y24" s="445"/>
+      <c r="Z24" s="443">
         <v>1.17</v>
       </c>
-      <c r="AA24" s="448"/>
-      <c r="AB24" s="449"/>
-      <c r="AC24" s="450"/>
-      <c r="AD24" s="451"/>
-      <c r="AE24" s="452"/>
+      <c r="AA24" s="444"/>
+      <c r="AB24" s="445"/>
+      <c r="AC24" s="446"/>
+      <c r="AD24" s="447"/>
+      <c r="AE24" s="448"/>
       <c r="AF24" s="44"/>
       <c r="AG24" s="44"/>
       <c r="AH24" s="44"/>
@@ -19417,9 +19413,9 @@
       <c r="Z27" s="388"/>
       <c r="AA27" s="389"/>
       <c r="AB27" s="390"/>
-      <c r="AC27" s="453"/>
-      <c r="AD27" s="454"/>
-      <c r="AE27" s="455"/>
+      <c r="AC27" s="449"/>
+      <c r="AD27" s="450"/>
+      <c r="AE27" s="451"/>
       <c r="AF27" s="44"/>
       <c r="AG27" s="44"/>
       <c r="AH27" s="44"/>
@@ -19534,22 +19530,22 @@
       <c r="Q29" s="13"/>
       <c r="R29" s="13"/>
       <c r="S29" s="13"/>
-      <c r="T29" s="456">
+      <c r="T29" s="452">
         <v>14614</v>
       </c>
-      <c r="U29" s="457"/>
-      <c r="V29" s="458"/>
-      <c r="W29" s="456"/>
-      <c r="X29" s="457"/>
-      <c r="Y29" s="458"/>
-      <c r="Z29" s="459">
+      <c r="U29" s="453"/>
+      <c r="V29" s="454"/>
+      <c r="W29" s="452"/>
+      <c r="X29" s="453"/>
+      <c r="Y29" s="454"/>
+      <c r="Z29" s="455">
         <v>39350</v>
       </c>
-      <c r="AA29" s="460"/>
-      <c r="AB29" s="461"/>
-      <c r="AC29" s="450"/>
-      <c r="AD29" s="451"/>
-      <c r="AE29" s="452"/>
+      <c r="AA29" s="456"/>
+      <c r="AB29" s="457"/>
+      <c r="AC29" s="446"/>
+      <c r="AD29" s="447"/>
+      <c r="AE29" s="448"/>
       <c r="AF29" s="44"/>
       <c r="AG29" s="44"/>
       <c r="AH29" s="44"/>
@@ -19664,23 +19660,23 @@
       <c r="Q31" s="13"/>
       <c r="R31" s="13"/>
       <c r="S31" s="13"/>
-      <c r="T31" s="447">
+      <c r="T31" s="443">
         <f>Z23</f>
         <v>3.4830000000000001</v>
       </c>
-      <c r="U31" s="448"/>
-      <c r="V31" s="449"/>
+      <c r="U31" s="444"/>
+      <c r="V31" s="445"/>
       <c r="W31" s="424"/>
       <c r="X31" s="425"/>
       <c r="Y31" s="426"/>
-      <c r="Z31" s="447">
+      <c r="Z31" s="443">
         <v>17.527999999999999</v>
       </c>
-      <c r="AA31" s="448"/>
-      <c r="AB31" s="449"/>
-      <c r="AC31" s="450"/>
-      <c r="AD31" s="451"/>
-      <c r="AE31" s="452"/>
+      <c r="AA31" s="444"/>
+      <c r="AB31" s="445"/>
+      <c r="AC31" s="446"/>
+      <c r="AD31" s="447"/>
+      <c r="AE31" s="448"/>
       <c r="AF31" s="45"/>
       <c r="AG31" s="44"/>
       <c r="AH31" s="44"/>
@@ -19726,22 +19722,22 @@
       <c r="Q32" s="13"/>
       <c r="R32" s="13"/>
       <c r="S32" s="13"/>
-      <c r="T32" s="447">
+      <c r="T32" s="443">
         <v>10.44</v>
       </c>
-      <c r="U32" s="448"/>
-      <c r="V32" s="449"/>
+      <c r="U32" s="444"/>
+      <c r="V32" s="445"/>
       <c r="W32" s="424"/>
       <c r="X32" s="425"/>
       <c r="Y32" s="426"/>
-      <c r="Z32" s="447">
+      <c r="Z32" s="443">
         <v>75.44</v>
       </c>
-      <c r="AA32" s="448"/>
-      <c r="AB32" s="449"/>
-      <c r="AC32" s="450"/>
-      <c r="AD32" s="451"/>
-      <c r="AE32" s="452"/>
+      <c r="AA32" s="444"/>
+      <c r="AB32" s="445"/>
+      <c r="AC32" s="446"/>
+      <c r="AD32" s="447"/>
+      <c r="AE32" s="448"/>
       <c r="AF32" s="45"/>
       <c r="AG32" s="44"/>
       <c r="AH32" s="44"/>
@@ -19932,9 +19928,9 @@
       <c r="Z35" s="388"/>
       <c r="AA35" s="389"/>
       <c r="AB35" s="389"/>
-      <c r="AC35" s="450"/>
-      <c r="AD35" s="451"/>
-      <c r="AE35" s="452"/>
+      <c r="AC35" s="446"/>
+      <c r="AD35" s="447"/>
+      <c r="AE35" s="448"/>
       <c r="AF35" s="12"/>
       <c r="AG35" s="12"/>
       <c r="AH35" s="12"/>
@@ -19986,19 +19982,19 @@
       <c r="Q36" s="13"/>
       <c r="R36" s="13"/>
       <c r="S36" s="13"/>
-      <c r="T36" s="447">
+      <c r="T36" s="443">
         <v>636</v>
       </c>
-      <c r="U36" s="448"/>
-      <c r="V36" s="449"/>
+      <c r="U36" s="444"/>
+      <c r="V36" s="445"/>
       <c r="W36" s="389"/>
       <c r="X36" s="389"/>
       <c r="Y36" s="389"/>
-      <c r="Z36" s="447">
+      <c r="Z36" s="443">
         <v>7718</v>
       </c>
-      <c r="AA36" s="448"/>
-      <c r="AB36" s="449"/>
+      <c r="AA36" s="444"/>
+      <c r="AB36" s="445"/>
       <c r="AC36" s="53"/>
       <c r="AD36" s="48"/>
       <c r="AE36" s="48"/>
@@ -20114,17 +20110,17 @@
       <c r="Q38" s="13"/>
       <c r="R38" s="13"/>
       <c r="S38" s="13"/>
-      <c r="T38" s="447">
+      <c r="T38" s="443">
         <v>5162</v>
       </c>
-      <c r="U38" s="448"/>
-      <c r="V38" s="448"/>
-      <c r="W38" s="448"/>
-      <c r="X38" s="448"/>
-      <c r="Y38" s="448"/>
-      <c r="Z38" s="448"/>
-      <c r="AA38" s="448"/>
-      <c r="AB38" s="449"/>
+      <c r="U38" s="444"/>
+      <c r="V38" s="444"/>
+      <c r="W38" s="444"/>
+      <c r="X38" s="444"/>
+      <c r="Y38" s="444"/>
+      <c r="Z38" s="444"/>
+      <c r="AA38" s="444"/>
+      <c r="AB38" s="445"/>
       <c r="AC38" s="48"/>
       <c r="AD38" s="48"/>
       <c r="AE38" s="49"/>
@@ -20234,22 +20230,22 @@
       <c r="Q40" s="13"/>
       <c r="R40" s="13"/>
       <c r="S40" s="13"/>
-      <c r="T40" s="447">
+      <c r="T40" s="443">
         <v>34550</v>
       </c>
-      <c r="U40" s="448"/>
-      <c r="V40" s="449"/>
+      <c r="U40" s="444"/>
+      <c r="V40" s="445"/>
       <c r="W40" s="389"/>
       <c r="X40" s="389"/>
       <c r="Y40" s="389"/>
-      <c r="Z40" s="447">
+      <c r="Z40" s="443">
         <v>83420</v>
       </c>
-      <c r="AA40" s="448"/>
-      <c r="AB40" s="449"/>
-      <c r="AC40" s="450"/>
-      <c r="AD40" s="451"/>
-      <c r="AE40" s="452"/>
+      <c r="AA40" s="444"/>
+      <c r="AB40" s="445"/>
+      <c r="AC40" s="446"/>
+      <c r="AD40" s="447"/>
+      <c r="AE40" s="448"/>
       <c r="AF40" s="44"/>
       <c r="AG40" s="44"/>
       <c r="AH40" s="44"/>
@@ -20314,9 +20310,9 @@
       </c>
       <c r="AA41" s="496"/>
       <c r="AB41" s="497"/>
-      <c r="AC41" s="450"/>
-      <c r="AD41" s="451"/>
-      <c r="AE41" s="452"/>
+      <c r="AC41" s="446"/>
+      <c r="AD41" s="447"/>
+      <c r="AE41" s="448"/>
       <c r="AF41" s="44"/>
       <c r="AG41" s="44"/>
       <c r="AH41" s="44"/>
@@ -21640,27 +21636,27 @@
       </c>
       <c r="U61" s="75"/>
       <c r="V61" s="75"/>
-      <c r="W61" s="438">
+      <c r="W61" s="458">
         <v>0</v>
       </c>
-      <c r="X61" s="438"/>
-      <c r="Y61" s="438"/>
-      <c r="Z61" s="438"/>
-      <c r="AA61" s="438"/>
+      <c r="X61" s="458"/>
+      <c r="Y61" s="458"/>
+      <c r="Z61" s="458"/>
+      <c r="AA61" s="458"/>
       <c r="AB61" s="76" t="s">
         <v>2</v>
       </c>
       <c r="AC61" s="76"/>
       <c r="AD61" s="76"/>
-      <c r="AE61" s="438" t="s">
+      <c r="AE61" s="458" t="s">
         <v>82</v>
       </c>
-      <c r="AF61" s="438"/>
-      <c r="AG61" s="438"/>
-      <c r="AH61" s="438"/>
-      <c r="AI61" s="438"/>
-      <c r="AJ61" s="438"/>
-      <c r="AK61" s="438"/>
+      <c r="AF61" s="458"/>
+      <c r="AG61" s="458"/>
+      <c r="AH61" s="458"/>
+      <c r="AI61" s="458"/>
+      <c r="AJ61" s="458"/>
+      <c r="AK61" s="458"/>
       <c r="AL61" s="10"/>
       <c r="AM61" s="74"/>
       <c r="AN61" s="10"/>
@@ -21703,26 +21699,26 @@
       <c r="U62" s="75"/>
       <c r="V62" s="75"/>
       <c r="W62" s="76"/>
-      <c r="X62" s="439" t="s">
+      <c r="X62" s="459" t="s">
         <v>82</v>
       </c>
-      <c r="Y62" s="439"/>
-      <c r="Z62" s="439"/>
-      <c r="AA62" s="439"/>
+      <c r="Y62" s="459"/>
+      <c r="Z62" s="459"/>
+      <c r="AA62" s="459"/>
       <c r="AB62" s="81" t="s">
         <v>7</v>
       </c>
       <c r="AC62" s="81"/>
-      <c r="AD62" s="438" t="s">
+      <c r="AD62" s="458" t="s">
         <v>82</v>
       </c>
-      <c r="AE62" s="438"/>
-      <c r="AF62" s="438"/>
-      <c r="AG62" s="438"/>
-      <c r="AH62" s="438"/>
-      <c r="AI62" s="438"/>
-      <c r="AJ62" s="438"/>
-      <c r="AK62" s="438"/>
+      <c r="AE62" s="458"/>
+      <c r="AF62" s="458"/>
+      <c r="AG62" s="458"/>
+      <c r="AH62" s="458"/>
+      <c r="AI62" s="458"/>
+      <c r="AJ62" s="458"/>
+      <c r="AK62" s="458"/>
       <c r="AL62" s="10"/>
       <c r="AM62" s="74"/>
       <c r="AN62" s="10"/>
@@ -21939,14 +21935,14 @@
       <c r="H66" s="71"/>
       <c r="I66" s="71"/>
       <c r="J66" s="71"/>
-      <c r="K66" s="440" t="s">
+      <c r="K66" s="460" t="s">
         <v>87</v>
       </c>
-      <c r="L66" s="441"/>
-      <c r="M66" s="441"/>
-      <c r="N66" s="441"/>
-      <c r="O66" s="441"/>
-      <c r="P66" s="441"/>
+      <c r="L66" s="461"/>
+      <c r="M66" s="461"/>
+      <c r="N66" s="461"/>
+      <c r="O66" s="461"/>
+      <c r="P66" s="461"/>
       <c r="Q66" s="203" t="s">
         <v>88</v>
       </c>
@@ -22000,22 +21996,22 @@
       <c r="H67" s="96"/>
       <c r="I67" s="96"/>
       <c r="J67" s="96"/>
-      <c r="K67" s="444" t="s">
+      <c r="K67" s="440" t="s">
         <v>35</v>
       </c>
-      <c r="L67" s="445"/>
-      <c r="M67" s="446"/>
-      <c r="N67" s="444" t="s">
+      <c r="L67" s="441"/>
+      <c r="M67" s="442"/>
+      <c r="N67" s="440" t="s">
         <v>346</v>
       </c>
-      <c r="O67" s="445"/>
-      <c r="P67" s="446"/>
-      <c r="Q67" s="444" t="s">
+      <c r="O67" s="441"/>
+      <c r="P67" s="442"/>
+      <c r="Q67" s="440" t="s">
         <v>357</v>
       </c>
-      <c r="R67" s="445"/>
-      <c r="S67" s="445"/>
-      <c r="T67" s="446"/>
+      <c r="R67" s="441"/>
+      <c r="S67" s="441"/>
+      <c r="T67" s="442"/>
       <c r="U67" s="97"/>
       <c r="V67" s="98" t="s">
         <v>90</v>
@@ -22031,17 +22027,17 @@
         <v>92</v>
       </c>
       <c r="AC67" s="99"/>
-      <c r="AD67" s="442" t="s">
+      <c r="AD67" s="438" t="s">
         <v>93</v>
       </c>
-      <c r="AE67" s="443"/>
-      <c r="AF67" s="443"/>
-      <c r="AG67" s="443"/>
-      <c r="AH67" s="443"/>
-      <c r="AI67" s="443"/>
-      <c r="AJ67" s="443"/>
-      <c r="AK67" s="443"/>
-      <c r="AL67" s="443"/>
+      <c r="AE67" s="439"/>
+      <c r="AF67" s="439"/>
+      <c r="AG67" s="439"/>
+      <c r="AH67" s="439"/>
+      <c r="AI67" s="439"/>
+      <c r="AJ67" s="439"/>
+      <c r="AK67" s="439"/>
+      <c r="AL67" s="439"/>
       <c r="AM67" s="100"/>
       <c r="AN67" s="9"/>
       <c r="AO67" s="9"/>
@@ -28687,6 +28683,11 @@
     <mergeCell ref="T21:V21"/>
     <mergeCell ref="Z21:AB21"/>
     <mergeCell ref="AC21:AE21"/>
+    <mergeCell ref="W61:AA61"/>
+    <mergeCell ref="AE61:AK61"/>
+    <mergeCell ref="X62:AA62"/>
+    <mergeCell ref="AD62:AK62"/>
+    <mergeCell ref="K66:P66"/>
     <mergeCell ref="T23:V23"/>
     <mergeCell ref="Z23:AB23"/>
     <mergeCell ref="AC23:AE23"/>
@@ -28696,11 +28697,6 @@
     <mergeCell ref="AC17:AE17"/>
     <mergeCell ref="W20:Y20"/>
     <mergeCell ref="W18:Y18"/>
-    <mergeCell ref="K69:M69"/>
-    <mergeCell ref="N69:P69"/>
-    <mergeCell ref="B70:G70"/>
-    <mergeCell ref="K70:M70"/>
-    <mergeCell ref="N70:P70"/>
     <mergeCell ref="T24:V24"/>
     <mergeCell ref="Z24:AB24"/>
     <mergeCell ref="AC24:AE24"/>
@@ -28715,11 +28711,6 @@
     <mergeCell ref="T32:V32"/>
     <mergeCell ref="Z32:AB32"/>
     <mergeCell ref="AC32:AE32"/>
-    <mergeCell ref="W61:AA61"/>
-    <mergeCell ref="AE61:AK61"/>
-    <mergeCell ref="X62:AA62"/>
-    <mergeCell ref="AD62:AK62"/>
-    <mergeCell ref="K66:P66"/>
     <mergeCell ref="AD67:AL67"/>
     <mergeCell ref="K76:M76"/>
     <mergeCell ref="N76:P76"/>
@@ -28739,6 +28730,11 @@
     <mergeCell ref="N67:P67"/>
     <mergeCell ref="Q67:T67"/>
     <mergeCell ref="B69:G69"/>
+    <mergeCell ref="K69:M69"/>
+    <mergeCell ref="N69:P69"/>
+    <mergeCell ref="B70:G70"/>
+    <mergeCell ref="K70:M70"/>
+    <mergeCell ref="N70:P70"/>
     <mergeCell ref="X119:AA119"/>
     <mergeCell ref="AD119:AK119"/>
     <mergeCell ref="AH155:AK155"/>
@@ -30032,10 +30028,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:AG50"/>
+  <dimension ref="B2:AB50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AD23" sqref="AD23"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="U57" sqref="U57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30058,8 +30054,8 @@
     <col min="28" max="28" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="2:33" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:21" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="512" t="s">
         <v>296</v>
       </c>
@@ -30096,7 +30092,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="4" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="514" t="s">
         <v>359</v>
       </c>
@@ -30127,7 +30123,7 @@
       <c r="T4" s="535"/>
       <c r="U4" s="595"/>
     </row>
-    <row r="5" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="514" t="s">
         <v>319</v>
       </c>
@@ -30174,7 +30170,7 @@
       </c>
       <c r="S5" s="592"/>
     </row>
-    <row r="6" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="514" t="s">
         <v>96</v>
       </c>
@@ -30221,7 +30217,7 @@
       </c>
       <c r="S6" s="593"/>
     </row>
-    <row r="7" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B7" s="514" t="s">
         <v>97</v>
       </c>
@@ -30271,41 +30267,8 @@
       <c r="S7" s="381">
         <v>1.196678766955152</v>
       </c>
-      <c r="W7">
-        <v>21002.326409887686</v>
-      </c>
-      <c r="X7">
-        <v>6000</v>
-      </c>
-      <c r="Y7">
-        <v>88</v>
-      </c>
-      <c r="Z7">
-        <v>40</v>
-      </c>
-      <c r="AA7">
-        <v>224</v>
-      </c>
-      <c r="AB7">
-        <v>78</v>
-      </c>
-      <c r="AC7">
-        <v>116672.5292608053</v>
-      </c>
-      <c r="AD7">
-        <v>12847.158290277126</v>
-      </c>
-      <c r="AE7">
-        <v>40</v>
-      </c>
-      <c r="AF7">
-        <v>1500</v>
-      </c>
-      <c r="AG7">
-        <v>125</v>
-      </c>
     </row>
-    <row r="8" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B8" s="514" t="s">
         <v>98</v>
       </c>
@@ -30355,41 +30318,8 @@
       <c r="S8" s="380">
         <v>1.1456757934618682</v>
       </c>
-      <c r="W8">
-        <v>29619.8226853753</v>
-      </c>
-      <c r="X8">
-        <v>8000</v>
-      </c>
-      <c r="Y8">
-        <v>93</v>
-      </c>
-      <c r="Z8">
-        <v>40</v>
-      </c>
-      <c r="AA8">
-        <v>224</v>
-      </c>
-      <c r="AB8">
-        <v>74</v>
-      </c>
-      <c r="AC8">
-        <v>155563.3723477404</v>
-      </c>
-      <c r="AD8">
-        <v>17129.544387036167</v>
-      </c>
-      <c r="AE8">
-        <v>40</v>
-      </c>
-      <c r="AF8">
-        <v>1360</v>
-      </c>
-      <c r="AG8">
-        <v>120</v>
-      </c>
     </row>
-    <row r="9" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B9" s="514" t="s">
         <v>99</v>
       </c>
@@ -30439,41 +30369,8 @@
       <c r="S9" s="270">
         <v>1.0897330679057786</v>
       </c>
-      <c r="W9">
-        <v>35144.307786208119</v>
-      </c>
-      <c r="X9">
-        <v>9000</v>
-      </c>
-      <c r="Y9">
-        <v>98</v>
-      </c>
-      <c r="Z9">
-        <v>40</v>
-      </c>
-      <c r="AA9">
-        <v>224</v>
-      </c>
-      <c r="AB9">
-        <v>73</v>
-      </c>
-      <c r="AC9">
-        <v>175008.79389120796</v>
-      </c>
-      <c r="AD9">
-        <v>19270.737435415689</v>
-      </c>
-      <c r="AE9">
-        <v>40</v>
-      </c>
-      <c r="AF9">
-        <v>1260</v>
-      </c>
-      <c r="AG9">
-        <v>115</v>
-      </c>
     </row>
-    <row r="10" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B10" s="514" t="s">
         <v>100</v>
       </c>
@@ -30523,41 +30420,8 @@
       <c r="S10" s="270">
         <v>1.0190879189227857</v>
       </c>
-      <c r="W10">
-        <v>41889.463107497941</v>
-      </c>
-      <c r="X10">
-        <v>10000</v>
-      </c>
-      <c r="Y10">
-        <v>105</v>
-      </c>
-      <c r="Z10">
-        <v>40</v>
-      </c>
-      <c r="AA10">
-        <v>224</v>
-      </c>
-      <c r="AB10">
-        <v>72</v>
-      </c>
-      <c r="AC10">
-        <v>194454.21543467548</v>
-      </c>
-      <c r="AD10">
-        <v>21411.930483795208</v>
-      </c>
-      <c r="AE10">
-        <v>40</v>
-      </c>
-      <c r="AF10">
-        <v>1150</v>
-      </c>
-      <c r="AG10">
-        <v>112</v>
-      </c>
     </row>
-    <row r="11" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B11" s="514" t="s">
         <v>102</v>
       </c>
@@ -30607,41 +30471,8 @@
       <c r="S11" s="270">
         <v>0.97362491092613601</v>
       </c>
-      <c r="W11">
-        <v>46755.510190508096</v>
-      </c>
-      <c r="X11">
-        <v>10645</v>
-      </c>
-      <c r="Y11">
-        <v>110</v>
-      </c>
-      <c r="Z11">
-        <v>40</v>
-      </c>
-      <c r="AA11">
-        <v>224</v>
-      </c>
-      <c r="AB11">
-        <v>71.450773994121278</v>
-      </c>
-      <c r="AC11">
-        <v>206996.51233021205</v>
-      </c>
-      <c r="AD11">
-        <v>22793</v>
-      </c>
-      <c r="AE11">
-        <v>40</v>
-      </c>
-      <c r="AF11">
-        <v>1159</v>
-      </c>
-      <c r="AG11">
-        <v>112.41819933258614</v>
-      </c>
     </row>
-    <row r="12" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B12" s="514" t="s">
         <v>295</v>
       </c>
@@ -30691,41 +30522,8 @@
       <c r="S12" s="270">
         <v>0.80217780579342823</v>
       </c>
-      <c r="W12">
-        <v>69851.180978331904</v>
-      </c>
-      <c r="X12">
-        <v>13000</v>
-      </c>
-      <c r="Y12">
-        <v>134</v>
-      </c>
-      <c r="Z12">
-        <v>40</v>
-      </c>
-      <c r="AA12">
-        <v>224</v>
-      </c>
-      <c r="AB12">
-        <v>69</v>
-      </c>
-      <c r="AC12">
-        <v>252790.48006507813</v>
-      </c>
-      <c r="AD12">
-        <v>27835.509628933771</v>
-      </c>
-      <c r="AE12">
-        <v>40</v>
-      </c>
-      <c r="AF12">
-        <v>980</v>
-      </c>
-      <c r="AG12">
-        <v>110</v>
-      </c>
     </row>
-    <row r="13" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B13" s="514" t="s">
         <v>104</v>
       </c>
@@ -30750,7 +30548,7 @@
       <c r="R13" s="376"/>
       <c r="S13" s="270"/>
     </row>
-    <row r="14" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B14" s="514" t="s">
         <v>105</v>
       </c>
@@ -30775,7 +30573,7 @@
       <c r="R14" s="376"/>
       <c r="S14" s="270"/>
     </row>
-    <row r="15" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B15" s="514" t="s">
         <v>106</v>
       </c>
@@ -30800,7 +30598,7 @@
       <c r="R15" s="376"/>
       <c r="S15" s="270"/>
     </row>
-    <row r="16" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="514" t="s">
         <v>107</v>
       </c>

</xml_diff>